<commit_message>
Added public and private routes
</commit_message>
<xml_diff>
--- a/public/Sample.xlsx
+++ b/public/Sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>productName</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>quantity</t>
-  </si>
-  <si>
-    <t>userID</t>
   </si>
   <si>
     <t>ratings</t>
@@ -374,20 +371,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="9" width="12.33203125" customWidth="1"/>
+    <col min="3" max="8" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,9 +408,6 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>